<commit_message>
Enable support to Prompt Caching and Amazon Nova models
</commit_message>
<xml_diff>
--- a/samples/contract-compliance-analysis/backend/guidelines/guidelines_example.xlsx
+++ b/samples/contract-compliance-analysis/backend/guidelines/guidelines_example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gdalves/dev/aee/ifood/anonymized/ifood-backend-anonym-draft/guidelines/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gdalves/dev/aee/ifood/blueprint_v2/backend/guidelines/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FAEB3C-AD55-144B-9ACC-A632C993EF0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93044F90-970F-454E-865D-277C486A2D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="37060" yWindow="2680" windowWidth="40460" windowHeight="24140" xr2:uid="{FD2DBF6C-2FF1-CD4F-A391-81725205B6E0}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{FD2DBF6C-2FF1-CD4F-A391-81725205B6E0}"/>
   </bookViews>
   <sheets>
     <sheet name="Taxonomy" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="530" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="249">
   <si>
     <t>Id</t>
   </si>
@@ -65,9 +65,6 @@
     <t>Fees</t>
   </si>
   <si>
-    <t>Invoicing and Payment</t>
-  </si>
-  <si>
     <t>Expenses</t>
   </si>
   <si>
@@ -98,9 +95,6 @@
     <t>Force Majeure</t>
   </si>
   <si>
-    <t>Compliance with Laws and Regulations</t>
-  </si>
-  <si>
     <t>Ethical Conduct and Anti-Corruption</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Replacement of Personnel</t>
   </si>
   <si>
-    <t>Non-Solicitation of Employees</t>
-  </si>
-  <si>
     <t>Background Checks and Security Clearances</t>
   </si>
   <si>
@@ -143,9 +134,6 @@
     <t>Arbitration or Litigation</t>
   </si>
   <si>
-    <t>Post-Termination Obligations</t>
-  </si>
-  <si>
     <t>Notices</t>
   </si>
   <si>
@@ -155,9 +143,6 @@
     <t>Waiver</t>
   </si>
   <si>
-    <t>Non-Solicitation and Non-Competition</t>
-  </si>
-  <si>
     <t>Non-Disparagement</t>
   </si>
   <si>
@@ -227,9 +212,6 @@
     <t>Neither Party shall be liable for any delay or failure to perform its obligations under this Agreement due to causes beyond its reasonable control, including, but not limited to, acts of God, acts of civil or military authority, fires, floods, earthquakes, riots, wars, terrorist acts, epidemics, or governmental restrictions ("Force Majeure Event"). In the event of a Force Majeure Event, the affected Party shall promptly notify the other Party, and the Parties shall work together in good faith to mitigate the effects of the Force Majeure Event and, if necessary, amend or terminate this Agreement.</t>
   </si>
   <si>
-    <t>Each Party shall comply with all applicable laws, regulations, and industry standards in the performance of its obligations under this Agreement.</t>
-  </si>
-  <si>
     <t>Each Party shall comply with all applicable anti-corruption laws, including, but not limited to, the U.S. Foreign Corrupt Practices Act and the UK Bribery Act, and shall not engage in any form of bribery, kickbacks, or other corrupt practices in connection with this Agreement.</t>
   </si>
   <si>
@@ -242,9 +224,6 @@
     <t>If Company reasonably objects to the performance or conduct of any of Service Provider's personnel assigned to perform the Services, Service Provider shall promptly replace such personnel with qualified and experienced replacements acceptable to Company.</t>
   </si>
   <si>
-    <t>During the term of this Agreement and for a period of [X] years thereafter, neither Party shall, directly or indirectly, solicit or attempt to solicit for employment or engagement any employee or contractor of the other Party who was involved in the performance of this Agreement, without the prior written consent of the other Party.</t>
-  </si>
-  <si>
     <t>Service Provider shall ensure that all of its employees, agents, and subcontractors assigned to perform Services under this Agreement have successfully completed background checks and obtained any necessary security clearances as required by Company or applicable laws and regulations.</t>
   </si>
   <si>
@@ -272,9 +251,6 @@
     <t>If the dispute cannot be resolved through mediation, either Party may pursue binding arbitration in accordance with the rules of [Arbitration Service Provider], or, if the Parties mutually agree, may pursue litigation in a court of competent jurisdiction.</t>
   </si>
   <si>
-    <t>Upon termination or expiration of this Agreement, each Party shall promptly return or destroy (and certify such destruction) all Confidential Information and other materials belonging to the other Party, and Service Provider shall cooperate with Company to ensure an orderly transition of the Services to Company or a third-party service provider.</t>
-  </si>
-  <si>
     <t>All notices, requests, consents, claims, demands, waivers, and other communications under this Agreement shall be in writing and shall be deemed to have been duly given: (a) when delivered by hand (with written confirmation of receipt); (b) when received by the addressee if sent by a nationally recognized overnight courier (receipt requested); (c) on the date sent by email (with confirmation of transmission) if sent during normal business hours of the recipient, and on the next business day if sent after normal business hours of the recipient; or (d) on the third day after the date mailed, by certified or registered mail, return receipt requested, postage prepaid.</t>
   </si>
   <si>
@@ -452,15 +428,6 @@
     <t>Neither Party shall be liable for any delay or failure to perform its obligations under this Agreement due to causes beyond its reasonable control, including, but not limited to, acts of God, acts of civil or military authority, fires, floods, earthquakes, riots, wars, terrorist acts, epidemics, or governmental restrictions ("Force Majeure Event"). In the event of a Force Majeure Event, the affected Party shall promptly notify the other Party, and the Parties shall work together in good faith to mitigate the effects of the Force Majeure Event, which may include implementing contingency plans, adjusting service levels, or modifying the scope of services.</t>
   </si>
   <si>
-    <t>Service Provider shall comply with all applicable laws, regulations, and industry standards in the development and implementation of the ERP software system, including but not limited to data privacy laws, security standards, and software licensing requirements.</t>
-  </si>
-  <si>
-    <t>Both Parties shall comply with all applicable laws, regulations, and industry standards related to advertising and marketing practices, including but not limited to consumer protection laws, data privacy regulations, and truth-in-advertising principles.</t>
-  </si>
-  <si>
-    <t>Service Provider shall perform the facility management services in compliance with all applicable laws, regulations, and industry standards, including but not limited to environmental regulations, occupational health and safety standards, and building codes.</t>
-  </si>
-  <si>
     <t>Each Party shall conduct its business activities in an ethical manner and shall comply with all applicable anti-corruption laws, including but not limited to the U.S. Foreign Corrupt Practices Act and the UK Bribery Act. Neither Party shall offer, give, or accept any bribes, kickbacks, or other improper payments or benefits in connection with this Agreement.</t>
   </si>
   <si>
@@ -497,15 +464,6 @@
     <t>If Company reasonably objects to the performance or conduct of any of Service Provider's personnel assigned to the facility management services, Service Provider shall promptly replace such personnel with qualified and experienced replacements acceptable to Company.</t>
   </si>
   <si>
-    <t>During the term of this Agreement and for a period of 2 years thereafter, neither Party shall, directly or indirectly, solicit or attempt to solicit for employment or engagement any employee or contractor of the other Party who was involved in the performance of this Agreement, without the prior written consent of the other Party.</t>
-  </si>
-  <si>
-    <t>During the term of this Agreement and for a period of 1 year thereafter, neither Party shall, directly or indirectly, solicit or attempt to solicit for employment or engagement any employee or contractor of the other Party who was involved in the planning, execution, or management of the marketing and advertising campaigns, without the prior written consent of the other Party.</t>
-  </si>
-  <si>
-    <t>During the term of this Agreement and for a period of 18 months thereafter, neither Party shall, directly or indirectly, solicit or attempt to solicit for employment or engagement any employee or contractor of the other Party who was involved in the provision or management of the facility management services, without the prior written consent of the other Party.</t>
-  </si>
-  <si>
     <t>Service Provider shall ensure that all of its employees, agents, and subcontractors assigned to perform software development services under this Agreement have successfully completed background checks and obtained any necessary security clearances as required by Company or applicable laws and regulations, particularly for projects involving sensitive or confidential data.</t>
   </si>
   <si>
@@ -566,15 +524,6 @@
     <t>If the Parties are unable to resolve the dispute through negotiations within 30 days, the Parties shall submit the dispute to non-binding mediation in accordance with the rules of the American Arbitration Association.</t>
   </si>
   <si>
-    <t>Upon termination or expiration of this Agreement, Service Provider shall promptly deliver to Company all Deliverables, work in progress, and other materials related to the software development services, including but not limited to source code, documentation, and data. Service Provider shall also cooperate with Company to ensure an orderly transition of the software development activities to Company or a third-party service provider.</t>
-  </si>
-  <si>
-    <t>Upon termination or expiration of this Agreement, Service Provider shall promptly deliver to Company all creative assets, campaign data, and other materials related to the marketing and advertising services. Service Provider shall also cooperate with Company to ensure an orderly transition of the marketing and advertising activities to Company or a third-party service provider.</t>
-  </si>
-  <si>
-    <t>Upon termination or expiration of this Agreement, Service Provider shall promptly deliver to Company all facility records, documentation, and other materials related to the facility management services. Service Provider shall also cooperate with Company to ensure an orderly transition of the facility management activities to Company or a third-party service provider.</t>
-  </si>
-  <si>
     <t>During the term of this Agreement and for a period of 1 year thereafter, neither Party shall make any disparaging or defamatory statements, whether written or oral, regarding the other Party or its products, services, employees, or business practices.</t>
   </si>
   <si>
@@ -587,9 +536,6 @@
     <t>This clause may not be applicable or necessary for typical facility management services, unless the services are being provided in multiple countries or regions, in which case Service Provider shall ensure that the pricing, terms, and conditions offered to Company are at least as favorable as those offered to any other client or nation for similar services during the term of this Agreement.</t>
   </si>
   <si>
-    <t>Each Party shall cooperate with and provide reasonable assistance to the other Party in connection with the performance of its obligations under this Agreement, including but not limited to providing access to necessary information, systems, and personnel.</t>
-  </si>
-  <si>
     <t>This Agreement, together with the Statement of Work and any other exhibits or attachments, constitutes the entire agreement between the Parties with respect to the subject matter hereof and supersedes all prior agreements, understandings, and negotiations, both written and oral, between the Parties with respect to the subject matter of this Agreement. This Agreement may be amended or modified only by a written instrument duly executed by authorized representatives of both Parties.</t>
   </si>
   <si>
@@ -605,15 +551,6 @@
     <t>If the dispute cannot be resolved through mediation, either Party may pursue binding arbitration in accordance with the rules of the International Centre for Dispute Resolution, or, if the Parties mutually agree, may pursue litigation in a court of competent jurisdiction.</t>
   </si>
   <si>
-    <t>In the event of any dispute or disagreement arising out of or relating to this Agreement, the Parties shall first attempt to resolve the dispute through good faith negotiations between their respective executive-level representatives</t>
-  </si>
-  <si>
-    <t>In the event of any dispute or disagreement arising out of or relating to this Agreement, the Parties shall first attempt to resolve the dispute through good faith negotiations between their respective project managers or designated representatives</t>
-  </si>
-  <si>
-    <t>In the event of any dispute or disagreement arising out of or relating to this Agreement, the Parties shall first attempt to resolve the dispute through good faith negotiations between their respective legal representatives or in-house counsel</t>
-  </si>
-  <si>
     <t>All notices, requests, consents, claims, demands, waivers, and other communications under this Agreement shall be in writing and shall be deemed to have been duly given: (i) when delivered by hand (with written confirmation of receipt); (ii) when received by the addressee if sent by a nationally recognized overnight courier (receipt requested); (iii) on the date sent by email (with confirmation of transmission) if sent during normal business hours of the recipient, and on the next business day if sent after normal business hours of the recipient; or (iv) on the third day after the date mailed, by certified or registered mail, return receipt requested, postage prepaid, to the respective addresses of the Parties set forth in this Agreement or such other address as may be designated by a Party in accordance with this Section.</t>
   </si>
   <si>
@@ -635,12 +572,6 @@
     <t>The failure of either Party to insist upon or enforce strict performance of any provision of this Agreement, or to exercise any right or remedy to which it is entitled under this Agreement, shall not constitute a waiver of such provision, right, or remedy, and shall not cause a diminution of the obligations established by this Agreement. No waiver of any provision of this Agreement shall be effective unless it is in writing and signed by an authorized representative of the waiving Party, and any such waiver shall be effective only in the specific instance and for the purpose for which it is given.</t>
   </si>
   <si>
-    <t>During the term of this Agreement and for a period of 18 months following its termination or expiration, neither Party shall, directly or indirectly, solicit or hire any employee or contractor of the other Party who was involved in the performance of the services under this Agreement. Additionally, Service Provider shall not, during the term of this Agreement, engage in any business or activity that competes with the services provided to Company under this Agreement within a 50-mile radius of Company's principal place of business.</t>
-  </si>
-  <si>
-    <t>For a period of 3 years following the termination or expiration of this Agreement, neither Party shall, directly or indirectly, solicit or attempt to solicit for employment or engagement any employee or contractor of the other Party who was involved in the performance of this Agreement, without the prior written consent of the other Party. Additionally, Service Provider agrees not to engage in any business or activity that directly competes with the services provided to Company under this Agreement during the term of this Agreement and for a period of 1 year thereafter.</t>
-  </si>
-  <si>
     <t>Each Party agrees that, during the term of this Agreement and for a period of 2 years following its termination or expiration, it shall not make any negative, disparaging, or derogatory statements, whether written or oral, about the other Party, its products, services, employees, or business practices, to any third party, including but not limited to any customers, clients, or members of the public.</t>
   </si>
   <si>
@@ -651,33 +582,6 @@
   </si>
   <si>
     <t>Neither Party shall use the other Party's name, logo, trademarks, or other intellectual property in any publicity, advertising, or marketing materials, or for any other promotional purposes, without the prior written consent of the other Party. Notwithstanding the foregoing, Company shall have the right to use and display the Deliverables and any work product resulting from the services provided under this Agreement for internal business purposes and demonstrations to potential customers or investors.</t>
-  </si>
-  <si>
-    <t>The Parties shall cooperate and provide reasonable assistance to each other in connection with the performance of their respective obligations under this Agreement. Such cooperation and assistance may include, but is not limited to, providing access to relevant information, data, systems, and personnel, as well as participating in meetings, conference calls, and other communications as reasonably requested by the other Party.</t>
-  </si>
-  <si>
-    <t>Each Party shall, at all times during the term of this Agreement, cooperate and provide reasonable assistance to the other Party in connection with the performance of its obligations under this Agreement, including but not limited to providing access to necessary information, systems, and personnel, as well as responding promptly to reasonable requests for information or clarification. The Parties shall work together in good faith to facilitate the successful performance of their respective obligations under this Agreement.</t>
-  </si>
-  <si>
-    <t>The Parties acknowledge and agree that their relationship under this Agreement is that of independent contractors. Nothing in this Agreement shall be construed as creating an employer-employee relationship, partnership, joint venture, or agency relationship between the Parties. Neither Party shall have the authority to bind or obligate the other Party in any way, except as expressly set forth in this Agreement.</t>
-  </si>
-  <si>
-    <t>In performing their respective obligations under this Agreement, the Parties are and shall remain independent contractors. Nothing in this Agreement shall be construed as creating an employer-employee relationship, partnership, joint venture, or agency relationship between the Parties. Neither Party shall have the authority to act on behalf of or bind the other Party in any manner whatsoever, except as expressly set forth in this Agreement.</t>
-  </si>
-  <si>
-    <t>This Agreement, including all exhibits, schedules, and attachments hereto, constitutes the entire agreement between the Parties with respect to the subject matter hereof and supersedes all prior agreements, understandings, and negotiations, both written and oral, between the Parties with respect to the subject matter of this Agreement. No amendment, modification, or supplement to this Agreement shall be binding unless it is in writing and signed by authorized representatives of both Parties.</t>
-  </si>
-  <si>
-    <t>This Agreement, together with any addenda, exhibits, or other attachments expressly incorporated herein, constitutes the entire agreement between the Parties with respect to the subject matter hereof and supersedes all prior agreements, understandings, and negotiations, both written and oral, between the Parties with respect to the subject matter of this Agreement. This Agreement may be amended, modified, or supplemented only by a written instrument duly executed by authorized representatives of both Parties, which expressly references this Agreement and states the intention of the Parties to amend, modify, or supplement it.</t>
-  </si>
-  <si>
-    <t>This Agreement shall be governed by and construed in accordance with the laws of the State of California, without regard to its conflict of laws principles. The Parties hereby submit to the exclusive jurisdiction of the courts located in Los Angeles County, California for any legal proceedings arising out of or relating to this Agreement.</t>
-  </si>
-  <si>
-    <t>This Agreement shall be governed by and interpreted in accordance with the laws of the State of New York, without giving effect to its principles of conflict of laws. Any dispute, controversy, or claim arising out of or relating to this Agreement, or the breach, termination, or validity thereof, shall be subject to the exclusive jurisdiction of the courts located in New York County, New York.</t>
-  </si>
-  <si>
-    <t>This Agreement and any disputes arising out of or relating to this Agreement shall be governed by and construed in accordance with the laws of the State of Texas, without regard to its conflict of laws rules. The Parties irrevocably consent to the exclusive jurisdiction and venue of the state and federal courts located in Harris County, Texas for any legal proceedings arising out of or relating to this Agreement.</t>
   </si>
   <si>
     <t>Standard Wording</t>
@@ -819,14 +723,6 @@
 Does the clause mention the UK Bribery Act?</t>
   </si>
   <si>
-    <t>Does the clause mention that the parties must comply with applicable laws and regulations?
-Does the clause specify that the laws and regulations relate to corporate social responsibility?
-Does the clause include environmental protection as one of the areas covered by corporate social responsibility?
-Does the clause include labor practices as one of the areas covered by corporate social responsibility?
-Does the clause include human rights as one of the areas covered by corporate social responsibility?
-Does the clause indicate that the listed areas (environmental protection, labor practices, and human rights) are not an exhaustive list of areas covered by corporate social responsibility?</t>
-  </si>
-  <si>
     <t>Does the clause require the Service Provider to assign personnel to perform the Services?
 Does the clause specify that the personnel assigned must be qualified and experienced?
 Does the clause require the Service Provider to allocate sufficient resources to meet the requirements and timelines set forth in the Statement of Work?
@@ -877,13 +773,6 @@
 Does the clause specify a time period (in days) for the parties to attempt negotiations before proceeding further?
 Does the clause mention the parties submitting the dispute to non-binding mediation if negotiations fail?
 Does the clause reference the rules of a specific mediation service provider?</t>
-  </si>
-  <si>
-    <t>Does the clause mention mediation as a step before pursuing binding arbitration or litigation?
-Does the clause state that binding arbitration can be pursued if the dispute cannot be resolved through mediation?
-Does the clause specify that the binding arbitration should be in accordance with the rules of an Arbitration Service Provider?
-Does the clause indicate that litigation in a court of competent jurisdiction can be pursued if the parties mutually agree?
-Does the clause mention that either party may pursue binding arbitration or litigation?</t>
   </si>
   <si>
     <t>Does the clause specify that all communications under the agreement must be in writing?
@@ -918,13 +807,6 @@
 Does the clause apply the prohibition of using the other party's name, logo, or trademarks without prior written consent to both parties?</t>
   </si>
   <si>
-    <t>Does the clause specify that the Service Provider must ensure that the fees and terms offered to the Company are at least as favorable as those offered to any other customer or nation for similar services?
-Is it stated in the clause that the requirement for the Service Provider to offer fees and terms at least as favorable as those offered to others is conditional on it being specified in the Statement of Work?
-Does the clause mention both fees and terms that the Service Provider must ensure are at least as favorable as those offered to others?
-Is the Company explicitly mentioned as the party to whom the Service Provider must offer fees and terms that are at least as favorable as those offered to others?
-Does the clause specify that the requirement applies to fees and terms offered for similar services, without further qualification?</t>
-  </si>
-  <si>
     <t>Does the clause mention that the parties involved are required to cooperate with each other?
 Does the clause state that the parties involved are required to provide assistance to each other?
 Does the clause specify that the cooperation and assistance are in connection with the performance of obligations under the agreement?
@@ -965,11 +847,6 @@
 Does the clause allow the receiving party to disclose the confidential information to its employees, agents, or contractors who have a need to know and are bound by confidentiality obligations at least as protective as those set forth in the clause?</t>
   </si>
   <si>
-    <t>Does the clause mention that the services are to be provided on an exclusive basis if specified in the Statement of Work?
-Does the clause prohibit the Service Provider from providing similar services to third parties during the term of the Agreement?
-Does the clause specify that providing similar services to third parties requires prior written consent from the Company?</t>
-  </si>
-  <si>
     <t>Does the clause mention that it applies in case of any dispute or disagreement related to the agreement?
 Does the clause state that the parties involved must first try to resolve the dispute?
 Does the clause specify that the parties must attempt to resolve the dispute through good faith negotiations?</t>
@@ -995,6 +872,72 @@
     <t>Does the contract clause state that the agreement, together with the Statement of Work and any other exhibits or attachments, constitutes the entire agreement between the Parties with respect to the subject matter?
 Does the contract clause state that the agreement supersedes all prior agreements, understandings, and negotiations, both written and oral, between the Parties with respect to the subject matter of the agreement?
 Does the contract clause state that the agreement may be amended or modified only by a written instrument duly executed by authorized representatives of both Parties?</t>
+  </si>
+  <si>
+    <t>In the event of any dispute or disagreement arising out of or relating to this Agreement, the Parties shall first attempt to resolve the dispute through good faith negotiations between their respective executive-level representatives</t>
+  </si>
+  <si>
+    <t>In the event of any dispute or disagreement arising out of or relating to this Agreement, the Parties shall first attempt to resolve the dispute through good faith negotiations between their respective project managers or designated representatives</t>
+  </si>
+  <si>
+    <t>In the event of any dispute or disagreement arising out of or relating to this Agreement, the Parties shall first attempt to resolve the dispute through good faith negotiations between their respective legal representatives or in-house counsel</t>
+  </si>
+  <si>
+    <t>Each Party shall cooperate with and provide reasonable assistance to the other Party in connection with the performance of its obligations under this Agreement, including but not limited to providing access to necessary information, systems, and personnel.</t>
+  </si>
+  <si>
+    <t>The Parties shall cooperate and provide reasonable assistance to each other in connection with the performance of their respective obligations under this Agreement. Such cooperation and assistance may include, but is not limited to, providing access to relevant information, data, systems, and personnel, as well as participating in meetings, conference calls, and other communications as reasonably requested by the other Party.</t>
+  </si>
+  <si>
+    <t>Each Party shall, at all times during the term of this Agreement, cooperate and provide reasonable assistance to the other Party in connection with the performance of its obligations under this Agreement, including but not limited to providing access to necessary information, systems, and personnel, as well as responding promptly to reasonable requests for information or clarification. The Parties shall work together in good faith to facilitate the successful performance of their respective obligations under this Agreement.</t>
+  </si>
+  <si>
+    <t>The Parties acknowledge and agree that their relationship under this Agreement is that of independent contractors. Nothing in this Agreement shall be construed as creating an employer-employee relationship, partnership, joint venture, or agency relationship between the Parties. Neither Party shall have the authority to bind or obligate the other Party in any way, except as expressly set forth in this Agreement.</t>
+  </si>
+  <si>
+    <t>In performing their respective obligations under this Agreement, the Parties are and shall remain independent contractors. Nothing in this Agreement shall be construed as creating an employer-employee relationship, partnership, joint venture, or agency relationship between the Parties. Neither Party shall have the authority to act on behalf of or bind the other Party in any manner whatsoever, except as expressly set forth in this Agreement.</t>
+  </si>
+  <si>
+    <t>This Agreement, including all exhibits, schedules, and attachments hereto, constitutes the entire agreement between the Parties with respect to the subject matter hereof and supersedes all prior agreements, understandings, and negotiations, both written and oral, between the Parties with respect to the subject matter of this Agreement. No amendment, modification, or supplement to this Agreement shall be binding unless it is in writing and signed by authorized representatives of both Parties.</t>
+  </si>
+  <si>
+    <t>This Agreement, together with any addenda, exhibits, or other attachments expressly incorporated herein, constitutes the entire agreement between the Parties with respect to the subject matter hereof and supersedes all prior agreements, understandings, and negotiations, both written and oral, between the Parties with respect to the subject matter of this Agreement. This Agreement may be amended, modified, or supplemented only by a written instrument duly executed by authorized representatives of both Parties, which expressly references this Agreement and states the intention of the Parties to amend, modify, or supplement it.</t>
+  </si>
+  <si>
+    <t>This Agreement shall be governed by and construed in accordance with the laws of the State of California, without regard to its conflict of laws principles. The Parties hereby submit to the exclusive jurisdiction of the courts located in Los Angeles County, California for any legal proceedings arising out of or relating to this Agreement.</t>
+  </si>
+  <si>
+    <t>This Agreement shall be governed by and interpreted in accordance with the laws of the State of New York, without giving effect to its principles of conflict of laws. Any dispute, controversy, or claim arising out of or relating to this Agreement, or the breach, termination, or validity thereof, shall be subject to the exclusive jurisdiction of the courts located in New York County, New York.</t>
+  </si>
+  <si>
+    <t>This Agreement and any disputes arising out of or relating to this Agreement shall be governed by and construed in accordance with the laws of the State of Texas, without regard to its conflict of laws rules. The Parties irrevocably consent to the exclusive jurisdiction and venue of the state and federal courts located in Harris County, Texas for any legal proceedings arising out of or relating to this Agreement.</t>
+  </si>
+  <si>
+    <t>Does the clause mention that the parties must comply with applicable laws and regulations?
+Does the clause specify that the laws and regulations relate to corporate social responsibility?
+Does the clause include environmental protection as one of the areas covered by corporate social responsibility?
+Does the clause include labor practices as one of the areas covered by corporate social responsibility?
+Does the clause include human rights as one of the areas covered by corporate social responsibility?</t>
+  </si>
+  <si>
+    <t>Each Party shall comply with corporate social responsibility laws and standards specific to environmental protection, labor practices, and human rights, and shall implement policies promoting sustainable operations, ethical employment practices, and community welfare.</t>
+  </si>
+  <si>
+    <t>Does the clause mention that the services are to be provided on an exclusive basis if specified in the Statement of Work?
+Does the clause prohibit the Service Provider from delivering similar services to third parties when the Statement of Work specifies exclusivity?
+Does the clause specify that providing similar services to third parties requires prior written consent from the Company?</t>
+  </si>
+  <si>
+    <t>Does the clause specify that the Service Provider must ensure that the fees and terms offered to the Company are at least as favorable as those offered to any other customer or nation for similar services?
+Is it stated in the clause that the requirement for the Service Provider to offer fees and terms at least as favorable as those offered to others is conditional on it being specified in the Statement of Work?
+Does the clause mention both fees and terms that the Service Provider must ensure are at least as favorable as those offered to others?
+Is the Company explicitly mentioned as the party to whom the Service Provider must offer fees and terms that are at least as favorable as those offered to others?</t>
+  </si>
+  <si>
+    <t>Does the clause mention mediation as a step before pursuing binding arbitration or litigation?
+Does the clause state that binding arbitration can be pursued if the dispute cannot be resolved through mediation?
+Does the clause specify that the binding arbitration should be in accordance with the rules of a recognized arbitration organization?
+Does the clause indicate that litigation in a court of competent jurisdiction can be pursued if the parties mutually agree?</t>
   </si>
 </sst>
 </file>
@@ -1043,10 +986,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1076,9 +1019,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1116,7 +1059,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1222,7 +1165,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1364,7 +1307,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1374,8 +1317,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2763079-711B-9546-BF78-5DCA270CA6BA}">
   <dimension ref="A1:H42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1392,22 +1337,22 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C1" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="E1" t="s">
-        <v>265</v>
+        <v>229</v>
       </c>
       <c r="F1" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="G1" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="H1" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1418,13 +1363,13 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="E2" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1435,13 +1380,13 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="E3" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1452,13 +1397,13 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="E4" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1469,13 +1414,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="E5" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F5" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1486,13 +1431,13 @@
         <v>5</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
       <c r="E6" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="F6" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1503,13 +1448,13 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="E7" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F7" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1520,13 +1465,13 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E8" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="F8" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1534,16 +1479,16 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="C9" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F9" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1551,16 +1496,16 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E10" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F10" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1568,16 +1513,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E11" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F11" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1585,16 +1530,16 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E12" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="F12" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1602,16 +1547,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E13" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F13" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1619,16 +1564,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E14" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="F14" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1636,16 +1581,16 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>258</v>
+        <v>223</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1653,16 +1598,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F16" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1670,16 +1615,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="E17" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F17" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1687,16 +1632,16 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E18" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="F18" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1704,16 +1649,16 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="E19" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F19" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1721,16 +1666,16 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="E20" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F20" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1738,16 +1683,16 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>245</v>
       </c>
       <c r="E21" t="s">
-        <v>263</v>
-      </c>
-      <c r="F21" t="s">
-        <v>236</v>
+        <v>227</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1755,16 +1700,16 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E22" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F22" t="s">
-        <v>237</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1772,16 +1717,16 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="E23" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F23" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1789,16 +1734,16 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F24" t="s">
-        <v>239</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1806,16 +1751,16 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
       <c r="E25" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F25" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1823,16 +1768,16 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="E26" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F26" t="s">
-        <v>241</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1840,16 +1785,16 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>71</v>
+        <v>64</v>
       </c>
       <c r="E27" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1857,16 +1802,16 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
       <c r="E28" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F28" t="s">
-        <v>242</v>
+        <v>209</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1874,16 +1819,16 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="E29" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="F29" t="s">
-        <v>243</v>
+        <v>210</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1891,16 +1836,16 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C30" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="E30" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>260</v>
+        <v>224</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1908,16 +1853,16 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C31" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="E31" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="F31" s="1" t="s">
-        <v>244</v>
+        <v>211</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1925,16 +1870,16 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="E32" t="s">
-        <v>263</v>
-      </c>
-      <c r="F32" t="s">
-        <v>245</v>
+        <v>227</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1942,16 +1887,16 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C33" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="E33" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="F33" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1959,16 +1904,16 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C34" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E34" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="F34" t="s">
-        <v>247</v>
+        <v>213</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1976,16 +1921,16 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C35" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="E35" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="F35" t="s">
-        <v>248</v>
+        <v>214</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -1993,16 +1938,16 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C36" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="E36" t="s">
-        <v>264</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>261</v>
+        <v>228</v>
+      </c>
+      <c r="F36" s="3" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2010,16 +1955,16 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="C37" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="E37" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="F37" t="s">
-        <v>249</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2027,16 +1972,16 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="C38" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="E38" t="s">
-        <v>263</v>
-      </c>
-      <c r="F38" t="s">
-        <v>250</v>
+        <v>227</v>
+      </c>
+      <c r="F38" s="1" t="s">
+        <v>247</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2044,16 +1989,16 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C39" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="E39" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F39" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2061,16 +2006,16 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>255</v>
+        <v>220</v>
       </c>
       <c r="C40" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="E40" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="F40" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2078,16 +2023,16 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="C41" t="s">
-        <v>183</v>
+        <v>165</v>
       </c>
       <c r="E41" t="s">
-        <v>263</v>
+        <v>227</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>266</v>
+        <v>230</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.2">
@@ -2095,16 +2040,16 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
       <c r="E42" t="s">
-        <v>262</v>
+        <v>226</v>
       </c>
       <c r="F42" s="1" t="s">
-        <v>257</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -2125,10 +2070,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349ED4EB-C9CD-0B4B-96B9-1DCF4E02A0F8}">
-  <dimension ref="A1:C179"/>
+  <dimension ref="A1:C163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2140,13 +2085,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2157,7 +2102,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2168,7 +2113,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2179,7 +2124,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2190,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -2201,7 +2146,7 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -2212,7 +2157,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -2223,7 +2168,7 @@
         <v>2</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -2234,7 +2179,7 @@
         <v>2</v>
       </c>
       <c r="C9" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -2245,7 +2190,7 @@
         <v>3</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -2256,7 +2201,7 @@
         <v>3</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -2267,7 +2212,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -2278,7 +2223,7 @@
         <v>3</v>
       </c>
       <c r="C13" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -2289,7 +2234,7 @@
         <v>4</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -2300,7 +2245,7 @@
         <v>4</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -2311,7 +2256,7 @@
         <v>4</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -2322,7 +2267,7 @@
         <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -2333,7 +2278,7 @@
         <v>5</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -2344,7 +2289,7 @@
         <v>5</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -2355,7 +2300,7 @@
         <v>5</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="68" x14ac:dyDescent="0.2">
@@ -2366,7 +2311,7 @@
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>253</v>
+        <v>218</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -2377,7 +2322,7 @@
         <v>6</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -2388,7 +2333,7 @@
         <v>6</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -2399,7 +2344,7 @@
         <v>6</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -2410,7 +2355,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -2421,7 +2366,7 @@
         <v>7</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -2432,7 +2377,7 @@
         <v>7</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -2443,7 +2388,7 @@
         <v>7</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -2454,733 +2399,733 @@
         <v>7</v>
       </c>
       <c r="C29" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="2" t="s">
-        <v>8</v>
+      <c r="A30" t="s">
+        <v>219</v>
       </c>
       <c r="B30">
         <v>8</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="2" t="s">
-        <v>8</v>
+      <c r="A31" t="s">
+        <v>219</v>
       </c>
       <c r="B31">
         <v>8</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="2" t="s">
-        <v>8</v>
+      <c r="A32" t="s">
+        <v>219</v>
       </c>
       <c r="B32">
         <v>8</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>254</v>
+        <v>219</v>
       </c>
       <c r="B33">
         <v>8</v>
       </c>
       <c r="C33" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B34">
         <v>9</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B35">
         <v>9</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36">
         <v>9</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B37">
         <v>9</v>
       </c>
       <c r="C37" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B38">
         <v>10</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B39">
         <v>10</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B40">
         <v>10</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B41">
         <v>10</v>
       </c>
       <c r="C41" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42">
         <v>11</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43">
         <v>11</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B44">
         <v>11</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B45">
         <v>11</v>
       </c>
       <c r="C45" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B46">
         <v>12</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B47">
         <v>12</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B48">
         <v>12</v>
       </c>
       <c r="C48" s="2" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B49">
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B50">
         <v>13</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B51">
         <v>13</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B52">
         <v>13</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B53">
         <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B54">
         <v>14</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>184</v>
+        <v>166</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B55">
         <v>14</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>185</v>
+        <v>167</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B56">
         <v>14</v>
       </c>
       <c r="C56" s="2" t="s">
-        <v>186</v>
+        <v>168</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B57">
         <v>14</v>
       </c>
       <c r="C57" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B58">
         <v>15</v>
       </c>
       <c r="C58" s="2" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B59">
         <v>15</v>
       </c>
       <c r="C59" s="2" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B60">
         <v>15</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B61">
         <v>15</v>
       </c>
       <c r="C61" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B62">
         <v>16</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B63">
         <v>16</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B64">
         <v>16</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B65">
         <v>16</v>
       </c>
       <c r="C65" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B66">
         <v>17</v>
       </c>
       <c r="C66" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B67">
         <v>17</v>
       </c>
       <c r="C67" s="2" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B68">
         <v>17</v>
       </c>
       <c r="C68" s="2" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B69">
         <v>17</v>
       </c>
       <c r="C69" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B70">
         <v>18</v>
       </c>
       <c r="C70" s="2" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B71">
         <v>18</v>
       </c>
       <c r="C71" s="2" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B72">
         <v>18</v>
       </c>
       <c r="C72" s="2" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B73">
         <v>18</v>
       </c>
       <c r="C73" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B74">
         <v>19</v>
       </c>
       <c r="C74" s="2" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B75">
         <v>19</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B76">
         <v>19</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B77">
         <v>19</v>
       </c>
       <c r="C77" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B78">
         <v>20</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B79">
         <v>20</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B80">
         <v>20</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B81">
         <v>20</v>
       </c>
       <c r="C81" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B82">
         <v>21</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B83">
         <v>21</v>
       </c>
       <c r="C83" s="2" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B84">
         <v>21</v>
       </c>
       <c r="C84" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B85">
         <v>21</v>
       </c>
       <c r="C85" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B86">
         <v>22</v>
       </c>
       <c r="C86" s="2" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B87">
         <v>22</v>
       </c>
       <c r="C87" s="2" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B88">
         <v>22</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B89">
         <v>22</v>
       </c>
       <c r="C89" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B90">
         <v>23</v>
       </c>
       <c r="C90" s="2" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B91">
         <v>23</v>
       </c>
       <c r="C91" s="2" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B92">
         <v>23</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B93">
         <v>23</v>
       </c>
       <c r="C93" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="94" spans="1:3" ht="17" x14ac:dyDescent="0.2">
       <c r="A94" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B94">
         <v>24</v>
       </c>
-      <c r="C94" s="2" t="s">
-        <v>152</v>
+      <c r="C94" s="4" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="2" t="s">
-        <v>24</v>
+      <c r="A95" t="s">
+        <v>23</v>
       </c>
       <c r="B95">
         <v>24</v>
       </c>
-      <c r="C95" s="2" t="s">
-        <v>153</v>
+      <c r="C95" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
@@ -3188,43 +3133,43 @@
         <v>24</v>
       </c>
       <c r="B96">
+        <v>25</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="C96" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" t="s">
-        <v>24</v>
-      </c>
       <c r="B97">
-        <v>24</v>
-      </c>
-      <c r="C97" t="s">
-        <v>67</v>
+        <v>25</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B98">
         <v>25</v>
       </c>
       <c r="C98" s="2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B99">
         <v>25</v>
       </c>
-      <c r="C99" s="2" t="s">
-        <v>156</v>
+      <c r="C99" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -3232,10 +3177,10 @@
         <v>25</v>
       </c>
       <c r="B100">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C100" s="2" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -3243,257 +3188,257 @@
         <v>25</v>
       </c>
       <c r="B101">
+        <v>26</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="C101" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="102" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A102" s="2" t="s">
-        <v>26</v>
       </c>
       <c r="B102">
         <v>26</v>
       </c>
-      <c r="C102" s="3" t="s">
-        <v>69</v>
+      <c r="C102" s="2" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B103">
         <v>26</v>
       </c>
       <c r="C103" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A104" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B104">
         <v>27</v>
       </c>
       <c r="C104" s="2" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B105">
         <v>27</v>
       </c>
       <c r="C105" s="2" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A106" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B106">
         <v>27</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B107">
         <v>27</v>
       </c>
       <c r="C107" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" t="s">
-        <v>28</v>
+      <c r="A108" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B108">
         <v>28</v>
       </c>
       <c r="C108" s="2" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" t="s">
-        <v>28</v>
+      <c r="A109" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B109">
         <v>28</v>
       </c>
       <c r="C109" s="2" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" t="s">
-        <v>28</v>
+      <c r="A110" s="2" t="s">
+        <v>27</v>
       </c>
       <c r="B110">
         <v>28</v>
       </c>
       <c r="C110" s="2" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B111">
         <v>28</v>
       </c>
       <c r="C111" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="2" t="s">
-        <v>29</v>
+      <c r="A112" t="s">
+        <v>28</v>
       </c>
       <c r="B112">
         <v>29</v>
       </c>
       <c r="C112" s="2" t="s">
-        <v>164</v>
+        <v>231</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="2" t="s">
-        <v>29</v>
+      <c r="A113" t="s">
+        <v>28</v>
       </c>
       <c r="B113">
         <v>29</v>
       </c>
       <c r="C113" s="2" t="s">
-        <v>165</v>
+        <v>232</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="2" t="s">
-        <v>29</v>
+      <c r="A114" t="s">
+        <v>28</v>
       </c>
       <c r="B114">
         <v>29</v>
       </c>
       <c r="C114" s="2" t="s">
-        <v>166</v>
+        <v>233</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B115">
         <v>29</v>
       </c>
       <c r="C115" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="2" t="s">
-        <v>30</v>
+      <c r="A116" t="s">
+        <v>29</v>
       </c>
       <c r="B116">
         <v>30</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="2" t="s">
-        <v>30</v>
+      <c r="A117" t="s">
+        <v>29</v>
       </c>
       <c r="B117">
         <v>30</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="2" t="s">
-        <v>30</v>
+      <c r="A118" t="s">
+        <v>29</v>
       </c>
       <c r="B118">
         <v>30</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B119">
         <v>30</v>
       </c>
       <c r="C119" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B120">
         <v>31</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>188</v>
+        <v>157</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B121">
         <v>31</v>
       </c>
       <c r="C121" s="2" t="s">
-        <v>189</v>
+        <v>159</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B122">
         <v>31</v>
       </c>
       <c r="C122" s="2" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B123">
         <v>31</v>
       </c>
       <c r="C123" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" t="s">
-        <v>32</v>
+      <c r="A124" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B124">
         <v>32</v>
@@ -3503,52 +3448,52 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" t="s">
-        <v>32</v>
+      <c r="A125" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B125">
         <v>32</v>
       </c>
       <c r="C125" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" t="s">
-        <v>32</v>
+      <c r="A126" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="B126">
         <v>32</v>
       </c>
       <c r="C126" s="2" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B127">
         <v>32</v>
       </c>
       <c r="C127" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" t="s">
-        <v>33</v>
+      <c r="A128" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B128">
         <v>33</v>
       </c>
       <c r="C128" s="2" t="s">
-        <v>171</v>
+        <v>71</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" t="s">
-        <v>33</v>
+      <c r="A129" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B129">
         <v>33</v>
@@ -3558,558 +3503,382 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" t="s">
-        <v>33</v>
+      <c r="A130" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="B130">
         <v>33</v>
       </c>
       <c r="C130" s="2" t="s">
-        <v>187</v>
+        <v>174</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B131">
         <v>33</v>
       </c>
       <c r="C131" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A132" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B132">
         <v>34</v>
       </c>
       <c r="C132" s="2" t="s">
-        <v>175</v>
+        <v>72</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A133" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B133">
         <v>34</v>
       </c>
       <c r="C133" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A134" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B134">
         <v>34</v>
       </c>
       <c r="C134" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B135">
         <v>34</v>
       </c>
       <c r="C135" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A136" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B136">
         <v>35</v>
       </c>
       <c r="C136" s="2" t="s">
-        <v>191</v>
+        <v>161</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A137" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B137">
         <v>35</v>
       </c>
       <c r="C137" s="2" t="s">
-        <v>192</v>
+        <v>177</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A138" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B138">
         <v>35</v>
       </c>
       <c r="C138" s="2" t="s">
-        <v>193</v>
+        <v>178</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B139">
         <v>35</v>
       </c>
       <c r="C139" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A140" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B140">
         <v>36</v>
       </c>
       <c r="C140" s="2" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A141" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B141">
         <v>36</v>
       </c>
       <c r="C141" s="2" t="s">
-        <v>194</v>
+        <v>179</v>
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A142" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B142">
         <v>36</v>
       </c>
       <c r="C142" s="2" t="s">
-        <v>195</v>
+        <v>180</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B143">
         <v>36</v>
       </c>
       <c r="C143" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A144" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B144">
         <v>37</v>
       </c>
       <c r="C144" s="2" t="s">
-        <v>80</v>
+        <v>162</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A145" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B145">
         <v>37</v>
       </c>
       <c r="C145" s="2" t="s">
-        <v>196</v>
+        <v>163</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A146" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B146">
         <v>37</v>
       </c>
       <c r="C146" s="2" t="s">
-        <v>197</v>
+        <v>164</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B147">
         <v>37</v>
       </c>
       <c r="C147" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A148" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B148">
         <v>38</v>
       </c>
       <c r="C148" s="2" t="s">
-        <v>152</v>
+        <v>234</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A149" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B149">
         <v>38</v>
       </c>
       <c r="C149" s="2" t="s">
-        <v>198</v>
+        <v>235</v>
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A150" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B150">
         <v>38</v>
       </c>
       <c r="C150" s="2" t="s">
-        <v>199</v>
+        <v>236</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
-        <v>38</v>
+      <c r="A151" s="2" t="s">
+        <v>37</v>
       </c>
       <c r="B151">
         <v>38</v>
       </c>
       <c r="C151" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A152" s="2" t="s">
-        <v>39</v>
+        <v>220</v>
       </c>
       <c r="B152">
         <v>39</v>
       </c>
       <c r="C152" s="2" t="s">
-        <v>178</v>
+        <v>77</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A153" s="2" t="s">
-        <v>39</v>
+        <v>220</v>
       </c>
       <c r="B153">
         <v>39</v>
       </c>
       <c r="C153" s="2" t="s">
-        <v>200</v>
+        <v>237</v>
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A154" s="2" t="s">
-        <v>39</v>
+        <v>220</v>
       </c>
       <c r="B154">
         <v>39</v>
       </c>
       <c r="C154" s="2" t="s">
-        <v>201</v>
+        <v>238</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
-        <v>39</v>
+      <c r="A155" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="B155">
         <v>39</v>
       </c>
       <c r="C155" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A156" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B156">
         <v>40</v>
       </c>
       <c r="C156" s="2" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A157" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B157">
         <v>40</v>
       </c>
       <c r="C157" s="2" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A158" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B158">
         <v>40</v>
       </c>
       <c r="C158" s="2" t="s">
-        <v>203</v>
+        <v>240</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
-        <v>40</v>
+      <c r="A159" s="2" t="s">
+        <v>38</v>
       </c>
       <c r="B159">
         <v>40</v>
       </c>
       <c r="C159" t="s">
-        <v>82</v>
+        <v>165</v>
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A160" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B160">
         <v>41</v>
       </c>
       <c r="C160" s="2" t="s">
-        <v>179</v>
+        <v>241</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A161" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B161">
         <v>41</v>
       </c>
       <c r="C161" s="2" t="s">
-        <v>180</v>
+        <v>242</v>
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A162" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B162">
         <v>41</v>
       </c>
       <c r="C162" s="2" t="s">
-        <v>181</v>
+        <v>243</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163" t="s">
-        <v>41</v>
+      <c r="A163" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="B163">
         <v>41</v>
       </c>
       <c r="C163" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B164">
-        <v>42</v>
-      </c>
-      <c r="C164" s="2" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B165">
-        <v>42</v>
-      </c>
-      <c r="C165" s="2" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="B166">
-        <v>42</v>
-      </c>
-      <c r="C166" s="2" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="167" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A167" t="s">
-        <v>42</v>
-      </c>
-      <c r="B167">
-        <v>42</v>
-      </c>
-      <c r="C167" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="168" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A168" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B168">
-        <v>43</v>
-      </c>
-      <c r="C168" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="169" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A169" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B169">
-        <v>43</v>
-      </c>
-      <c r="C169" s="2" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="170" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A170" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="B170">
-        <v>43</v>
-      </c>
-      <c r="C170" s="2" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="171" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A171" t="s">
-        <v>255</v>
-      </c>
-      <c r="B171">
-        <v>43</v>
-      </c>
-      <c r="C171" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A172" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B172">
-        <v>44</v>
-      </c>
-      <c r="C172" s="2" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="173" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A173" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B173">
-        <v>44</v>
-      </c>
-      <c r="C173" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="174" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A174" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B174">
-        <v>44</v>
-      </c>
-      <c r="C174" s="2" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A175" t="s">
-        <v>43</v>
-      </c>
-      <c r="B175">
-        <v>44</v>
-      </c>
-      <c r="C175" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A176" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B176">
-        <v>45</v>
-      </c>
-      <c r="C176" s="2" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B177">
-        <v>45</v>
-      </c>
-      <c r="C177" s="2" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A178" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B178">
-        <v>45</v>
-      </c>
-      <c r="C178" s="2" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179" t="s">
-        <v>44</v>
-      </c>
-      <c r="B179">
-        <v>45</v>
-      </c>
-      <c r="C179" t="s">
-        <v>256</v>
+        <v>221</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C179">
-    <sortCondition ref="B1:B179"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C163">
+    <sortCondition ref="B1:B163"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>